<commit_message>
discivered longscroll.js, implemented simple scroll bar but not infinite scrolling. Need to understand longscroll.js and implement that!
</commit_message>
<xml_diff>
--- a/schedule2019.xlsx
+++ b/schedule2019.xlsx
@@ -14,7 +14,7 @@
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sheet4!$AN$7:$AN$71</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sheet4!$AN$7:$AN$75</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="295">
   <si>
     <t>এই বছর এ  কি কি চাই ?</t>
   </si>
@@ -935,6 +935,45 @@
   </si>
   <si>
     <t>CodeForcesRound-574: Div2 (Problem-C analysis)</t>
+  </si>
+  <si>
+    <t>* Add Month, Year combobox</t>
+  </si>
+  <si>
+    <t>* Grid Generate by Month/Year</t>
+  </si>
+  <si>
+    <t>* Connect with a DataBase (Python OR MySQL DB)</t>
+  </si>
+  <si>
+    <t>* User signup/login/logout</t>
+  </si>
+  <si>
+    <t>* Show user's salat record from DB once login (default as current month from system)</t>
+  </si>
+  <si>
+    <t>TBD-1</t>
+  </si>
+  <si>
+    <t>*  Simple beautification and more professional look</t>
+  </si>
+  <si>
+    <t>* Database Design ---- JSON file for now for first 20 users</t>
+  </si>
+  <si>
+    <t>* Save user's salat record to DB ---- JSON</t>
+  </si>
+  <si>
+    <t>* Send to users to use and get feedback</t>
+  </si>
+  <si>
+    <t>* use the projec myself for a month and get a feel of what to improve</t>
+  </si>
+  <si>
+    <t>*  complete TBD-1 ---&gt; learn JS OOP, JS Design pattern, study and und longscroll.js</t>
+  </si>
+  <si>
+    <t>* Map with number of occurences as bubble combined with bottom part (x-axis) year, scroll/zoom year and it will show that year's occurences in map (source: data viz course 13 hours https://www.youtube.com/watch?v=_8V5o2UHG0E</t>
   </si>
 </sst>
 </file>
@@ -1788,7 +1827,7 @@
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <f ca="1">TODAY()</f>
-        <v>43664</v>
+        <v>43665</v>
       </c>
       <c r="U1" s="8" t="s">
         <v>96</v>
@@ -2919,10 +2958,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO76"/>
+  <dimension ref="A1:AQ76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AO24" sqref="AO24"/>
+    <sheetView tabSelected="1" topLeftCell="Z3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AK19" sqref="AK19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2934,7 +2973,7 @@
     <col min="22" max="22" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -2942,7 +2981,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -2950,7 +2989,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -2958,7 +2997,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -2966,7 +3005,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>174</v>
       </c>
@@ -3011,7 +3050,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>205</v>
       </c>
@@ -3056,7 +3095,7 @@
       </c>
       <c r="AO8" s="21"/>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>202</v>
       </c>
@@ -3065,7 +3104,7 @@
       </c>
       <c r="AO9" s="21"/>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>208</v>
       </c>
@@ -3081,8 +3120,11 @@
       <c r="AO10" s="21" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AQ10" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
       <c r="AI11" t="s">
         <v>223</v>
       </c>
@@ -3092,8 +3134,11 @@
       <c r="AO11" s="21" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AQ11" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>214</v>
       </c>
@@ -3106,30 +3151,43 @@
       <c r="AN12" s="20">
         <v>43665</v>
       </c>
-      <c r="AO12" s="21"/>
-    </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AO12" s="21" t="s">
+        <v>287</v>
+      </c>
+      <c r="AQ12" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>216</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>217</v>
       </c>
+      <c r="AI13" t="s">
+        <v>282</v>
+      </c>
       <c r="AO13" s="21"/>
-    </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AQ13" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>218</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>219</v>
       </c>
-      <c r="AI14" s="17" t="s">
-        <v>226</v>
-      </c>
-      <c r="AO14" s="21"/>
-    </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AI14" t="s">
+        <v>283</v>
+      </c>
+      <c r="AQ14" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>220</v>
       </c>
@@ -3137,15 +3195,19 @@
         <v>221</v>
       </c>
       <c r="AI15" t="s">
-        <v>227</v>
-      </c>
-      <c r="AO15" s="21"/>
-    </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+        <v>284</v>
+      </c>
+      <c r="AQ15" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
       <c r="AI16" t="s">
-        <v>228</v>
-      </c>
-      <c r="AO16" s="21"/>
+        <v>285</v>
+      </c>
+      <c r="AQ16" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="17" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
@@ -3179,17 +3241,13 @@
         <v>171</v>
       </c>
       <c r="W17" s="14"/>
-      <c r="AI17" t="s">
-        <v>229</v>
-      </c>
-      <c r="AO17" s="21"/>
     </row>
     <row r="18" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>189</v>
       </c>
-      <c r="AI18" t="s">
-        <v>230</v>
+      <c r="AI18" s="17" t="s">
+        <v>226</v>
       </c>
       <c r="AO18" s="21"/>
     </row>
@@ -3198,7 +3256,10 @@
         <v>195</v>
       </c>
       <c r="AI19" t="s">
-        <v>231</v>
+        <v>227</v>
+      </c>
+      <c r="AK19" t="s">
+        <v>294</v>
       </c>
       <c r="AO19" s="21"/>
     </row>
@@ -3207,10 +3268,7 @@
         <v>202</v>
       </c>
       <c r="AI20" t="s">
-        <v>253</v>
-      </c>
-      <c r="AN20" s="16">
-        <v>43664</v>
+        <v>228</v>
       </c>
       <c r="AO20" s="21"/>
     </row>
@@ -3221,14 +3279,17 @@
       <c r="B21" s="15" t="s">
         <v>207</v>
       </c>
+      <c r="AI21" t="s">
+        <v>229</v>
+      </c>
       <c r="AO21" s="21"/>
     </row>
     <row r="22" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>212</v>
       </c>
-      <c r="AI22" s="17" t="s">
-        <v>232</v>
+      <c r="AI22" t="s">
+        <v>230</v>
       </c>
       <c r="AO22" s="21"/>
     </row>
@@ -3240,10 +3301,7 @@
         <v>211</v>
       </c>
       <c r="AI23" t="s">
-        <v>233</v>
-      </c>
-      <c r="AN23" s="19">
-        <v>43664</v>
+        <v>231</v>
       </c>
       <c r="AO23" s="21"/>
     </row>
@@ -3252,9 +3310,9 @@
         <v>210</v>
       </c>
       <c r="AI24" t="s">
-        <v>234</v>
-      </c>
-      <c r="AN24" s="19">
+        <v>253</v>
+      </c>
+      <c r="AN24" s="16">
         <v>43664</v>
       </c>
       <c r="AO24" s="21"/>
@@ -3263,20 +3321,11 @@
       <c r="A25" t="s">
         <v>204</v>
       </c>
-      <c r="AI25" t="s">
-        <v>235</v>
-      </c>
-      <c r="AN25" s="20">
-        <v>43665</v>
-      </c>
       <c r="AO25" s="21"/>
     </row>
     <row r="26" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="AI26" t="s">
-        <v>236</v>
-      </c>
-      <c r="AN26" s="16">
-        <v>43666</v>
+      <c r="AI26" s="17" t="s">
+        <v>232</v>
       </c>
       <c r="AO26" s="21"/>
     </row>
@@ -3312,12 +3361,14 @@
         <v>172</v>
       </c>
       <c r="AI27" t="s">
-        <v>237</v>
-      </c>
-      <c r="AN27" s="16">
-        <v>43667</v>
-      </c>
-      <c r="AO27" s="21"/>
+        <v>233</v>
+      </c>
+      <c r="AN27" s="19">
+        <v>43664</v>
+      </c>
+      <c r="AO27" s="21" t="s">
+        <v>279</v>
+      </c>
     </row>
     <row r="28" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -3327,9 +3378,11 @@
         <v>176</v>
       </c>
       <c r="AI28" t="s">
-        <v>238</v>
-      </c>
-      <c r="AN28" s="16"/>
+        <v>234</v>
+      </c>
+      <c r="AN28" s="19">
+        <v>43664</v>
+      </c>
       <c r="AO28" s="21"/>
     </row>
     <row r="29" spans="1:41" x14ac:dyDescent="0.25">
@@ -3337,7 +3390,10 @@
         <v>177</v>
       </c>
       <c r="AI29" t="s">
-        <v>239</v>
+        <v>235</v>
+      </c>
+      <c r="AN29" s="20">
+        <v>43665</v>
       </c>
       <c r="AO29" s="21"/>
     </row>
@@ -3346,7 +3402,10 @@
         <v>178</v>
       </c>
       <c r="AI30" t="s">
-        <v>240</v>
+        <v>236</v>
+      </c>
+      <c r="AN30" s="16">
+        <v>43666</v>
       </c>
       <c r="AO30" s="21"/>
     </row>
@@ -3354,20 +3413,24 @@
       <c r="H31" t="s">
         <v>180</v>
       </c>
+      <c r="AI31" t="s">
+        <v>237</v>
+      </c>
+      <c r="AN31" s="16">
+        <v>43667</v>
+      </c>
       <c r="AO31" s="21"/>
     </row>
     <row r="32" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="AI32" s="17" t="s">
-        <v>242</v>
-      </c>
+      <c r="AI32" t="s">
+        <v>238</v>
+      </c>
+      <c r="AN32" s="16"/>
       <c r="AO32" s="21"/>
     </row>
     <row r="33" spans="1:41" x14ac:dyDescent="0.25">
       <c r="AI33" t="s">
-        <v>243</v>
-      </c>
-      <c r="AN33" s="18">
-        <v>43663</v>
+        <v>239</v>
       </c>
       <c r="AO33" s="21"/>
     </row>
@@ -3402,6 +3465,9 @@
       <c r="V34" s="14" t="s">
         <v>173</v>
       </c>
+      <c r="AI34" t="s">
+        <v>240</v>
+      </c>
       <c r="AO34" s="21"/>
     </row>
     <row r="35" spans="1:41" x14ac:dyDescent="0.25">
@@ -3411,12 +3477,6 @@
       <c r="H35" t="s">
         <v>179</v>
       </c>
-      <c r="AI35" s="17" t="s">
-        <v>244</v>
-      </c>
-      <c r="AJ35" s="15" t="s">
-        <v>246</v>
-      </c>
       <c r="AO35" s="21"/>
     </row>
     <row r="36" spans="1:41" x14ac:dyDescent="0.25">
@@ -3426,11 +3486,8 @@
       <c r="H36" t="s">
         <v>181</v>
       </c>
-      <c r="AI36" t="s">
-        <v>245</v>
-      </c>
-      <c r="AJ36" s="15" t="s">
-        <v>248</v>
+      <c r="AI36" s="17" t="s">
+        <v>242</v>
       </c>
       <c r="AO36" s="21"/>
     </row>
@@ -3442,10 +3499,10 @@
         <v>182</v>
       </c>
       <c r="AI37" t="s">
-        <v>247</v>
-      </c>
-      <c r="AJ37" s="15" t="s">
-        <v>250</v>
+        <v>243</v>
+      </c>
+      <c r="AN37" s="18">
+        <v>43663</v>
       </c>
       <c r="AO37" s="21"/>
     </row>
@@ -3453,20 +3510,17 @@
       <c r="A38" t="s">
         <v>187</v>
       </c>
-      <c r="AI38" t="s">
-        <v>249</v>
-      </c>
-      <c r="AJ38" s="15" t="s">
-        <v>252</v>
-      </c>
       <c r="AO38" s="21"/>
     </row>
     <row r="39" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>188</v>
       </c>
-      <c r="AI39" t="s">
-        <v>251</v>
+      <c r="AI39" s="17" t="s">
+        <v>244</v>
+      </c>
+      <c r="AJ39" s="15" t="s">
+        <v>246</v>
       </c>
       <c r="AO39" s="21"/>
     </row>
@@ -3474,20 +3528,29 @@
       <c r="A40" t="s">
         <v>196</v>
       </c>
+      <c r="AI40" t="s">
+        <v>245</v>
+      </c>
+      <c r="AJ40" s="15" t="s">
+        <v>248</v>
+      </c>
       <c r="AO40" s="21"/>
     </row>
     <row r="41" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="AI41" s="14" t="s">
-        <v>174</v>
+      <c r="AI41" t="s">
+        <v>247</v>
+      </c>
+      <c r="AJ41" s="15" t="s">
+        <v>250</v>
       </c>
       <c r="AO41" s="21"/>
     </row>
     <row r="42" spans="1:41" x14ac:dyDescent="0.25">
       <c r="AI42" t="s">
-        <v>256</v>
-      </c>
-      <c r="AN42" s="16">
-        <v>43666</v>
+        <v>249</v>
+      </c>
+      <c r="AJ42" s="15" t="s">
+        <v>252</v>
       </c>
       <c r="AO42" s="21"/>
     </row>
@@ -3523,14 +3586,9 @@
         <v>175</v>
       </c>
       <c r="AI43" t="s">
-        <v>266</v>
-      </c>
-      <c r="AN43" s="16">
-        <v>43674</v>
-      </c>
-      <c r="AO43" s="22">
-        <v>4.1666666666666664E-2</v>
-      </c>
+        <v>251</v>
+      </c>
+      <c r="AO43" s="21"/>
     </row>
     <row r="44" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
@@ -3539,15 +3597,7 @@
       <c r="H44" t="s">
         <v>198</v>
       </c>
-      <c r="AI44" t="s">
-        <v>257</v>
-      </c>
-      <c r="AN44" s="18">
-        <v>43663</v>
-      </c>
-      <c r="AO44" s="21" t="s">
-        <v>279</v>
-      </c>
+      <c r="AO44" s="21"/>
     </row>
     <row r="45" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
@@ -3556,11 +3606,8 @@
       <c r="H45" t="s">
         <v>199</v>
       </c>
-      <c r="AI45" t="s">
-        <v>258</v>
-      </c>
-      <c r="AN45" s="19">
-        <v>43664</v>
+      <c r="AI45" s="14" t="s">
+        <v>174</v>
       </c>
       <c r="AO45" s="21"/>
     </row>
@@ -3572,10 +3619,10 @@
         <v>200</v>
       </c>
       <c r="AI46" t="s">
-        <v>259</v>
-      </c>
-      <c r="AN46" s="20">
-        <v>43665</v>
+        <v>256</v>
+      </c>
+      <c r="AN46" s="16">
+        <v>43666</v>
       </c>
       <c r="AO46" s="21"/>
     </row>
@@ -3587,12 +3634,14 @@
         <v>201</v>
       </c>
       <c r="AI47" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="AN47" s="16">
-        <v>43666</v>
-      </c>
-      <c r="AO47" s="21"/>
+        <v>43674</v>
+      </c>
+      <c r="AO47" s="22">
+        <v>4.1666666666666664E-2</v>
+      </c>
     </row>
     <row r="48" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
@@ -3602,46 +3651,48 @@
         <v>197</v>
       </c>
       <c r="AI48" t="s">
-        <v>261</v>
-      </c>
-      <c r="AN48" s="16">
-        <v>43667</v>
-      </c>
-      <c r="AO48" s="21"/>
+        <v>257</v>
+      </c>
+      <c r="AN48" s="18">
+        <v>43663</v>
+      </c>
+      <c r="AO48" s="21" t="s">
+        <v>279</v>
+      </c>
     </row>
     <row r="49" spans="8:41" x14ac:dyDescent="0.25">
       <c r="AI49" t="s">
-        <v>262</v>
-      </c>
-      <c r="AN49" s="16">
-        <v>43668</v>
+        <v>258</v>
+      </c>
+      <c r="AN49" s="19">
+        <v>43664</v>
       </c>
       <c r="AO49" s="21"/>
     </row>
     <row r="50" spans="8:41" x14ac:dyDescent="0.25">
       <c r="AI50" t="s">
-        <v>263</v>
-      </c>
-      <c r="AN50" s="16">
-        <v>43669</v>
+        <v>259</v>
+      </c>
+      <c r="AN50" s="20">
+        <v>43665</v>
       </c>
       <c r="AO50" s="21"/>
     </row>
     <row r="51" spans="8:41" x14ac:dyDescent="0.25">
       <c r="AI51" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="AN51" s="16">
-        <v>43670</v>
+        <v>43666</v>
       </c>
       <c r="AO51" s="21"/>
     </row>
     <row r="52" spans="8:41" x14ac:dyDescent="0.25">
       <c r="AI52" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="AN52" s="16">
-        <v>43671</v>
+        <v>43667</v>
       </c>
       <c r="AO52" s="21"/>
     </row>
@@ -3659,10 +3710,10 @@
         <v>169</v>
       </c>
       <c r="AI53" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="AN53" s="16">
-        <v>43671</v>
+        <v>43668</v>
       </c>
       <c r="AO53" s="21"/>
     </row>
@@ -3675,7 +3726,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="AI54" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="AN54" s="16">
         <v>43669</v>
@@ -3691,14 +3742,12 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="AI55" t="s">
-        <v>280</v>
-      </c>
-      <c r="AN55" s="18">
-        <v>43663</v>
-      </c>
-      <c r="AO55" s="21" t="s">
-        <v>279</v>
-      </c>
+        <v>264</v>
+      </c>
+      <c r="AN55" s="16">
+        <v>43670</v>
+      </c>
+      <c r="AO55" s="21"/>
     </row>
     <row r="56" spans="8:41" x14ac:dyDescent="0.25">
       <c r="H56" s="16">
@@ -3709,78 +3758,80 @@
         <v>1</v>
       </c>
       <c r="AI56" t="s">
-        <v>281</v>
-      </c>
-      <c r="AN56" s="19">
-        <v>43664</v>
-      </c>
+        <v>265</v>
+      </c>
+      <c r="AN56" s="16">
+        <v>43671</v>
+      </c>
+      <c r="AO56" s="21"/>
     </row>
     <row r="57" spans="8:41" x14ac:dyDescent="0.25">
       <c r="H57" s="16">
         <v>43658</v>
       </c>
+      <c r="AI57" t="s">
+        <v>267</v>
+      </c>
+      <c r="AN57" s="16">
+        <v>43671</v>
+      </c>
       <c r="AO57" s="21"/>
     </row>
     <row r="58" spans="8:41" x14ac:dyDescent="0.25">
       <c r="H58" s="16">
         <v>43659</v>
       </c>
+      <c r="AI58" t="s">
+        <v>268</v>
+      </c>
+      <c r="AN58" s="16">
+        <v>43669</v>
+      </c>
       <c r="AO58" s="21"/>
     </row>
     <row r="59" spans="8:41" x14ac:dyDescent="0.25">
       <c r="H59" s="16">
         <v>43660</v>
       </c>
-      <c r="AI59" s="14" t="s">
-        <v>167</v>
-      </c>
-      <c r="AO59" s="21"/>
+      <c r="AI59" t="s">
+        <v>280</v>
+      </c>
+      <c r="AN59" s="18">
+        <v>43663</v>
+      </c>
+      <c r="AO59" s="21" t="s">
+        <v>279</v>
+      </c>
     </row>
     <row r="60" spans="8:41" x14ac:dyDescent="0.25">
       <c r="H60" s="16">
         <v>43661</v>
       </c>
       <c r="AI60" t="s">
-        <v>269</v>
-      </c>
-      <c r="AN60" s="16">
-        <v>43666</v>
-      </c>
-      <c r="AO60" s="21"/>
+        <v>281</v>
+      </c>
+      <c r="AN60" s="19">
+        <v>43664</v>
+      </c>
     </row>
     <row r="61" spans="8:41" x14ac:dyDescent="0.25">
       <c r="H61" s="16">
         <v>43662</v>
       </c>
-      <c r="AI61" t="s">
-        <v>270</v>
-      </c>
-      <c r="AN61" s="16">
-        <v>43666</v>
-      </c>
       <c r="AO61" s="21"/>
     </row>
     <row r="62" spans="8:41" x14ac:dyDescent="0.25">
       <c r="H62" s="16">
         <v>43663</v>
       </c>
-      <c r="AI62" t="s">
-        <v>278</v>
-      </c>
-      <c r="AN62" s="16">
-        <v>43667</v>
-      </c>
       <c r="AO62" s="21"/>
     </row>
     <row r="63" spans="8:41" x14ac:dyDescent="0.25">
       <c r="H63" s="16">
         <v>43664</v>
       </c>
-      <c r="AI63" t="s">
-        <v>271</v>
-      </c>
-      <c r="AN63" s="20">
-        <v>43665</v>
+      <c r="AI63" s="14" t="s">
+        <v>167</v>
       </c>
       <c r="AO63" s="21"/>
     </row>
@@ -3789,10 +3840,10 @@
         <v>43665</v>
       </c>
       <c r="AI64" t="s">
-        <v>272</v>
-      </c>
-      <c r="AN64" s="19">
-        <v>43664</v>
+        <v>269</v>
+      </c>
+      <c r="AN64" s="16">
+        <v>43666</v>
       </c>
       <c r="AO64" s="21"/>
     </row>
@@ -3801,10 +3852,10 @@
         <v>43666</v>
       </c>
       <c r="AI65" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="AN65" s="16">
-        <v>43667</v>
+        <v>43666</v>
       </c>
       <c r="AO65" s="21"/>
     </row>
@@ -3812,20 +3863,35 @@
       <c r="H66" s="16">
         <v>43667</v>
       </c>
+      <c r="AI66" t="s">
+        <v>278</v>
+      </c>
+      <c r="AN66" s="16">
+        <v>43667</v>
+      </c>
       <c r="AO66" s="21"/>
     </row>
     <row r="67" spans="8:41" x14ac:dyDescent="0.25">
       <c r="H67" s="16">
         <v>43668</v>
       </c>
+      <c r="AI67" t="s">
+        <v>271</v>
+      </c>
+      <c r="AN67" s="20">
+        <v>43665</v>
+      </c>
       <c r="AO67" s="21"/>
     </row>
     <row r="68" spans="8:41" x14ac:dyDescent="0.25">
       <c r="H68" s="16">
         <v>43669</v>
       </c>
-      <c r="AI68" s="14" t="s">
-        <v>273</v>
+      <c r="AI68" t="s">
+        <v>272</v>
+      </c>
+      <c r="AN68" s="19">
+        <v>43664</v>
       </c>
       <c r="AO68" s="21"/>
     </row>
@@ -3834,46 +3900,59 @@
         <v>43670</v>
       </c>
       <c r="AI69" t="s">
-        <v>274</v>
-      </c>
-      <c r="AN69" s="16"/>
+        <v>277</v>
+      </c>
+      <c r="AN69" s="16">
+        <v>43667</v>
+      </c>
       <c r="AO69" s="21"/>
     </row>
     <row r="70" spans="8:41" x14ac:dyDescent="0.25">
       <c r="H70" s="16">
         <v>43671</v>
       </c>
-      <c r="AI70" t="s">
-        <v>275</v>
-      </c>
+      <c r="AO70" s="21"/>
     </row>
     <row r="71" spans="8:41" x14ac:dyDescent="0.25">
       <c r="H71" s="16">
         <v>43672</v>
       </c>
-      <c r="AI71" t="s">
-        <v>276</v>
-      </c>
+      <c r="AO71" s="21"/>
     </row>
     <row r="72" spans="8:41" x14ac:dyDescent="0.25">
       <c r="H72" s="16">
         <v>43673</v>
       </c>
+      <c r="AI72" s="14" t="s">
+        <v>273</v>
+      </c>
+      <c r="AO72" s="21"/>
     </row>
     <row r="73" spans="8:41" x14ac:dyDescent="0.25">
       <c r="H73" s="16">
         <v>43674</v>
       </c>
+      <c r="AI73" t="s">
+        <v>274</v>
+      </c>
+      <c r="AN73" s="16"/>
+      <c r="AO73" s="21"/>
     </row>
     <row r="74" spans="8:41" x14ac:dyDescent="0.25">
       <c r="H74" s="16">
         <v>43675</v>
       </c>
+      <c r="AI74" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="75" spans="8:41" x14ac:dyDescent="0.25">
       <c r="H75" s="16">
         <v>43676</v>
       </c>
+      <c r="AI75" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="76" spans="8:41" x14ac:dyDescent="0.25">
       <c r="H76" s="16">
@@ -3881,7 +3960,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="AO8:AO55 AO57:AO69">
+  <conditionalFormatting sqref="AO61:AO73 AO8:AO13 AO18:AO59">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",AO8)))</formula>
     </cfRule>
@@ -3893,10 +3972,10 @@
     <hyperlink ref="B13" r:id="rId4"/>
     <hyperlink ref="B14" r:id="rId5"/>
     <hyperlink ref="B15" r:id="rId6"/>
-    <hyperlink ref="AJ35" r:id="rId7"/>
-    <hyperlink ref="AJ36" r:id="rId8"/>
-    <hyperlink ref="AJ37" r:id="rId9"/>
-    <hyperlink ref="AJ38" r:id="rId10"/>
+    <hyperlink ref="AJ39" r:id="rId7"/>
+    <hyperlink ref="AJ40" r:id="rId8"/>
+    <hyperlink ref="AJ41" r:id="rId9"/>
+    <hyperlink ref="AJ42" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId11"/>

</xml_diff>